<commit_message>
Fin de las funciones basicas
</commit_message>
<xml_diff>
--- a/beisbol_seguro/MySQL/Libro1.xlsx
+++ b/beisbol_seguro/MySQL/Libro1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>INSERT INTO  jugadores VALUES (</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Jolyn Christen</t>
+  </si>
+  <si>
+    <t>Promedio_bateo</t>
+  </si>
+  <si>
+    <t>Efectividad</t>
   </si>
 </sst>
 </file>
@@ -158,17 +164,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -444,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,10 +484,11 @@
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -487,11 +513,17 @@
       <c r="H1" t="s">
         <v>8</v>
       </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
       <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -499,34 +531,42 @@
         <v>20</v>
       </c>
       <c r="C2" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,9),$J$3,$K$3,$L$3,$M$3,$N$3,$O$3,$P$3,$Q$3,$R$3)</f>
-        <v>JARDINERO DERECHO</v>
+        <f ca="1">CHOOSE(RANDBETWEEN(1,9),$K$3,$L$3,$M$3,$N$3,$O$3,$P$3,$Q$3,$R$3,$S$3)</f>
+        <v>JARDINERO IZQUIERDO</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,20)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,20)</f>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F2">
-        <f ca="1">RANDBETWEEN(0,1)</f>
+        <f t="shared" ref="F2:F11" ca="1" si="0">RANDBETWEEN(0,1)</f>
         <v>1</v>
       </c>
       <c r="G2">
         <f ca="1">IF(F2=0,"NULL",RANDBETWEEN(1,20))</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2">
         <f ca="1">IF(F2=0,"NULL",RANDBETWEEN(1,20))</f>
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="str">
+        <f ca="1">IF(F2=0,SUBSTITUTE(TEXT(D2/E2,"0,00"),",","."),"NULL")</f>
+        <v>NULL</v>
+      </c>
+      <c r="J2" s="3" t="str">
+        <f ca="1">IF(F2=0,"NULL",SUBSTITUTE(TEXT(G2/H2*9,"0,00"),",","."))</f>
+        <v>9.82</v>
+      </c>
+      <c r="K2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -534,19 +574,19 @@
         <v>21</v>
       </c>
       <c r="C3" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,9),$J$3,$K$3,$L$3,$M$3,$N$3,$O$3,$P$3,$Q$3,$R$3)</f>
-        <v>RECEPTOR</v>
+        <f ca="1">CHOOSE(RANDBETWEEN(1,9),$K$3,$L$3,$M$3,$N$3,$O$3,$P$3,$Q$3,$R$3,$S$3)</f>
+        <v>PRIMERA BASE</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:E11" ca="1" si="0">RANDBETWEEN(1,20)</f>
-        <v>8</v>
+        <f t="shared" ref="D3:E11" ca="1" si="1">RANDBETWEEN(1,20)</f>
+        <v>5</v>
       </c>
       <c r="E3">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <f ca="1">RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
       <c r="G3" t="str">
@@ -557,35 +597,43 @@
         <f ca="1">IF(F3=0,"NULL",RANDBETWEEN(1,20))</f>
         <v>NULL</v>
       </c>
-      <c r="J3" t="s">
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I11" ca="1" si="2">IF(F3=0,SUBSTITUTE(TEXT(D3/E3,"0,00"),",","."),"NULL")</f>
+        <v>0.45</v>
+      </c>
+      <c r="J3" s="3" t="str">
+        <f t="shared" ref="J3:J11" ca="1" si="3">IF(F3=0,"NULL",SUBSTITUTE(TEXT(G3/H3*9,"0,00"),",","."))</f>
+        <v>NULL</v>
+      </c>
+      <c r="K3" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -593,31 +641,39 @@
         <v>22</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C11" ca="1" si="1">CHOOSE(RANDBETWEEN(1,9),$J$3,$K$3,$L$3,$M$3,$N$3,$O$3,$P$3,$Q$3,$R$3)</f>
+        <f t="shared" ref="C4:C11" ca="1" si="4">CHOOSE(RANDBETWEEN(1,9),$K$3,$L$3,$M$3,$N$3,$O$3,$P$3,$Q$3,$R$3,$S$3)</f>
         <v>TERCERA BASE</v>
       </c>
       <c r="D4">
+        <f t="shared" ca="1" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F11" ca="1" si="2">RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G11" ca="1" si="3">IF(F4=0,"NULL",RANDBETWEEN(1,20))</f>
+        <f t="shared" ref="G4:G11" ca="1" si="5">IF(F4=0,"NULL",RANDBETWEEN(1,20))</f>
         <v>NULL</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H11" ca="1" si="4">IF(F4=0,"NULL",RANDBETWEEN(1,20))</f>
-        <v>NULL</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H4:H11" ca="1" si="6">IF(F4=0,"NULL",RANDBETWEEN(1,20))</f>
+        <v>NULL</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.60</v>
+      </c>
+      <c r="J4" s="3" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>NULL</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -625,31 +681,39 @@
         <v>23</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>JARDINERO IZQUIERDO</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>JARDINERO CENTRAL</v>
       </c>
       <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>NULL</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>NULL</v>
+      </c>
+      <c r="I5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G5">
+        <v>0.88</v>
+      </c>
+      <c r="J5" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>NULL</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -657,31 +721,39 @@
         <v>24</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>PRIMERA BASE</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>LANZADOR</v>
       </c>
       <c r="D6">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>NULL</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>NULL</v>
+      </c>
+      <c r="I6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G6">
+        <v>6.00</v>
+      </c>
+      <c r="J6" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ca="1" si="4"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>NULL</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -689,31 +761,39 @@
         <v>25</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>TERCERA BASE</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>PRIMERA BASE</v>
       </c>
       <c r="D7">
+        <f t="shared" ca="1" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>NULL</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>NULL</v>
+      </c>
+      <c r="I7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G7" t="str">
+        <v>3.17</v>
+      </c>
+      <c r="J7" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>NULL</v>
       </c>
-      <c r="H7" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>NULL</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -721,31 +801,39 @@
         <v>26</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>CAMPOCORTO</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>PRIMERA BASE</v>
       </c>
       <c r="D8">
+        <f t="shared" ca="1" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G8" t="str">
+        <v>NULL</v>
+      </c>
+      <c r="J8" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>NULL</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>NULL</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -753,31 +841,39 @@
         <v>27</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>CAMPOCORTO</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>RECEPTOR</v>
       </c>
       <c r="D9">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="I9" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G9">
+        <v>NULL</v>
+      </c>
+      <c r="J9" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="H9">
-        <f t="shared" ca="1" si="4"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+        <v>18.00</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -785,31 +881,39 @@
         <v>28</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>TERCERA BASE</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>JARDINERO CENTRAL</v>
       </c>
       <c r="D10">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <f t="shared" ca="1" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>NULL</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>NULL</v>
+      </c>
+      <c r="I10" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G10" t="str">
+        <v>0.26</v>
+      </c>
+      <c r="J10" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>NULL</v>
       </c>
-      <c r="H10" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>NULL</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -817,31 +921,49 @@
         <v>29</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>PRIMERA BASE</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>LANZADOR</v>
       </c>
       <c r="D11">
+        <f t="shared" ca="1" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="E11">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>NULL</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>NULL</v>
+      </c>
+      <c r="I11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G11">
+        <v>1.18</v>
+      </c>
+      <c r="J11" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="H11">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>NULL</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F2:F11">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F11">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -851,73 +973,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A3:A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="101.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f ca="1">CONCATENATE(Hoja1!$J$2,Hoja1!A2,",","'",Hoja1!B2,"'",",","'",,Hoja1!C2,"'",",",Hoja1!D2,",",Hoja1!E2,",",Hoja1!F2,",",Hoja1!G2,",",Hoja1!H2,")")</f>
-        <v>INSERT INTO  jugadores VALUES (NULL,'Hildred Pettengill','JARDINERO DERECHO',9,15,1,13,16)</v>
+        <f ca="1">CONCATENATE(Hoja1!$K$2,Hoja1!A2,",","'",Hoja1!B2,"'",",","'",,Hoja1!C2,"'",",",Hoja1!D2,",",Hoja1!E2,",",Hoja1!F2,",",Hoja1!G2,",",Hoja1!H2,",",Hoja1!I2,",",Hoja1!J2,");")</f>
+        <v>INSERT INTO  jugadores VALUES (NULL,'Hildred Pettengill','JARDINERO IZQUIERDO',14,6,1,12,11,NULL,9.82);</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f ca="1">CONCATENATE(Hoja1!$J$2,Hoja1!A3,",","'",Hoja1!B3,"'",",","'",,Hoja1!C3,"'",",",Hoja1!D3,",",Hoja1!E3,",",Hoja1!F3,",",Hoja1!G3,",",Hoja1!H3,")")</f>
-        <v>INSERT INTO  jugadores VALUES (NULL,'Joe Mccrady','RECEPTOR',8,3,0,NULL,NULL)</v>
+        <f ca="1">CONCATENATE(Hoja1!$K$2,Hoja1!A3,",","'",Hoja1!B3,"'",",","'",,Hoja1!C3,"'",",",Hoja1!D3,",",Hoja1!E3,",",Hoja1!F3,",",Hoja1!G3,",",Hoja1!H3,",",Hoja1!I3,",",Hoja1!J3,");")</f>
+        <v>INSERT INTO  jugadores VALUES (NULL,'Joe Mccrady','PRIMERA BASE',5,11,0,NULL,NULL,0.45,NULL);</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f ca="1">CONCATENATE(Hoja1!$J$2,Hoja1!A4,",","'",Hoja1!B4,"'",",","'",,Hoja1!C4,"'",",",Hoja1!D4,",",Hoja1!E4,",",Hoja1!F4,",",Hoja1!G4,",",Hoja1!H4,")")</f>
-        <v>INSERT INTO  jugadores VALUES (NULL,'Debroah Cheshire','TERCERA BASE',2,17,0,NULL,NULL)</v>
+        <f ca="1">CONCATENATE(Hoja1!$K$2,Hoja1!A4,",","'",Hoja1!B4,"'",",","'",,Hoja1!C4,"'",",",Hoja1!D4,",",Hoja1!E4,",",Hoja1!F4,",",Hoja1!G4,",",Hoja1!H4,",",Hoja1!I4,",",Hoja1!J4,");")</f>
+        <v>INSERT INTO  jugadores VALUES (NULL,'Debroah Cheshire','TERCERA BASE',16,10,0,NULL,NULL,1.60,NULL);</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f ca="1">CONCATENATE(Hoja1!$J$2,Hoja1!A5,",","'",Hoja1!B5,"'",",","'",,Hoja1!C5,"'",",",Hoja1!D5,",",Hoja1!E5,",",Hoja1!F5,",",Hoja1!G5,",",Hoja1!H5,")")</f>
-        <v>INSERT INTO  jugadores VALUES (NULL,'Kasie Abshire','JARDINERO IZQUIERDO',18,5,1,3,1)</v>
+        <f ca="1">CONCATENATE(Hoja1!$K$2,Hoja1!A5,",","'",Hoja1!B5,"'",",","'",,Hoja1!C5,"'",",",Hoja1!D5,",",Hoja1!E5,",",Hoja1!F5,",",Hoja1!G5,",",Hoja1!H5,",",Hoja1!I5,",",Hoja1!J5,");")</f>
+        <v>INSERT INTO  jugadores VALUES (NULL,'Kasie Abshire','JARDINERO CENTRAL',15,17,0,NULL,NULL,0.88,NULL);</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f ca="1">CONCATENATE(Hoja1!$J$2,Hoja1!A6,",","'",Hoja1!B6,"'",",","'",,Hoja1!C6,"'",",",Hoja1!D6,",",Hoja1!E6,",",Hoja1!F6,",",Hoja1!G6,",",Hoja1!H6,")")</f>
-        <v>INSERT INTO  jugadores VALUES (NULL,'Lovie Larmon','PRIMERA BASE',4,4,1,19,13)</v>
+        <f ca="1">CONCATENATE(Hoja1!$K$2,Hoja1!A6,",","'",Hoja1!B6,"'",",","'",,Hoja1!C6,"'",",",Hoja1!D6,",",Hoja1!E6,",",Hoja1!F6,",",Hoja1!G6,",",Hoja1!H6,",",Hoja1!I6,",",Hoja1!J6,");")</f>
+        <v>INSERT INTO  jugadores VALUES (NULL,'Lovie Larmon','LANZADOR',6,1,0,NULL,NULL,6.00,NULL);</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f ca="1">CONCATENATE(Hoja1!$J$2,Hoja1!A7,",","'",Hoja1!B7,"'",",","'",,Hoja1!C7,"'",",",Hoja1!D7,",",Hoja1!E7,",",Hoja1!F7,",",Hoja1!G7,",",Hoja1!H7,")")</f>
-        <v>INSERT INTO  jugadores VALUES (NULL,'Treena Ghoston','TERCERA BASE',6,18,0,NULL,NULL)</v>
+        <f ca="1">CONCATENATE(Hoja1!$K$2,Hoja1!A7,",","'",Hoja1!B7,"'",",","'",,Hoja1!C7,"'",",",Hoja1!D7,",",Hoja1!E7,",",Hoja1!F7,",",Hoja1!G7,",",Hoja1!H7,",",Hoja1!I7,",",Hoja1!J7,");")</f>
+        <v>INSERT INTO  jugadores VALUES (NULL,'Treena Ghoston','PRIMERA BASE',19,6,0,NULL,NULL,3.17,NULL);</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f ca="1">CONCATENATE(Hoja1!$J$2,Hoja1!A8,",","'",Hoja1!B8,"'",",","'",,Hoja1!C8,"'",",",Hoja1!D8,",",Hoja1!E8,",",Hoja1!F8,",",Hoja1!G8,",",Hoja1!H8,")")</f>
-        <v>INSERT INTO  jugadores VALUES (NULL,'Mariam Harwell','CAMPOCORTO',2,6,0,NULL,NULL)</v>
+        <f ca="1">CONCATENATE(Hoja1!$K$2,Hoja1!A8,",","'",Hoja1!B8,"'",",","'",,Hoja1!C8,"'",",",Hoja1!D8,",",Hoja1!E8,",",Hoja1!F8,",",Hoja1!G8,",",Hoja1!H8,",",Hoja1!I8,",",Hoja1!J8,");")</f>
+        <v>INSERT INTO  jugadores VALUES (NULL,'Mariam Harwell','PRIMERA BASE',16,12,1,1,10,NULL,0.90);</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f ca="1">CONCATENATE(Hoja1!$J$2,Hoja1!A9,",","'",Hoja1!B9,"'",",","'",,Hoja1!C9,"'",",",Hoja1!D9,",",Hoja1!E9,",",Hoja1!F9,",",Hoja1!G9,",",Hoja1!H9,")")</f>
-        <v>INSERT INTO  jugadores VALUES (NULL,'Izetta Zaldivar','CAMPOCORTO',19,3,1,19,5)</v>
+        <f ca="1">CONCATENATE(Hoja1!$K$2,Hoja1!A9,",","'",Hoja1!B9,"'",",","'",,Hoja1!C9,"'",",",Hoja1!D9,",",Hoja1!E9,",",Hoja1!F9,",",Hoja1!G9,",",Hoja1!H9,",",Hoja1!I9,",",Hoja1!J9,");")</f>
+        <v>INSERT INTO  jugadores VALUES (NULL,'Izetta Zaldivar','RECEPTOR',11,17,1,4,2,NULL,18.00);</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f ca="1">CONCATENATE(Hoja1!$J$2,Hoja1!A10,",","'",Hoja1!B10,"'",",","'",,Hoja1!C10,"'",",",Hoja1!D10,",",Hoja1!E10,",",Hoja1!F10,",",Hoja1!G10,",",Hoja1!H10,")")</f>
-        <v>INSERT INTO  jugadores VALUES (NULL,'Alene Portillo','TERCERA BASE',9,13,0,NULL,NULL)</v>
+        <f ca="1">CONCATENATE(Hoja1!$K$2,Hoja1!A10,",","'",Hoja1!B10,"'",",","'",,Hoja1!C10,"'",",",Hoja1!D10,",",Hoja1!E10,",",Hoja1!F10,",",Hoja1!G10,",",Hoja1!H10,",",Hoja1!I10,",",Hoja1!J10,");")</f>
+        <v>INSERT INTO  jugadores VALUES (NULL,'Alene Portillo','JARDINERO CENTRAL',5,19,0,NULL,NULL,0.26,NULL);</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f ca="1">CONCATENATE(Hoja1!$J$2,Hoja1!A11,",","'",Hoja1!B11,"'",",","'",,Hoja1!C11,"'",",",Hoja1!D11,",",Hoja1!E11,",",Hoja1!F11,",",Hoja1!G11,",",Hoja1!H11,")")</f>
-        <v>INSERT INTO  jugadores VALUES (NULL,'Jolyn Christen','PRIMERA BASE',16,9,1,9,4)</v>
+        <f ca="1">CONCATENATE(Hoja1!$K$2,Hoja1!A11,",","'",Hoja1!B11,"'",",","'",,Hoja1!C11,"'",",",Hoja1!D11,",",Hoja1!E11,",",Hoja1!F11,",",Hoja1!G11,",",Hoja1!H11,",",Hoja1!I11,",",Hoja1!J11,");")</f>
+        <v>INSERT INTO  jugadores VALUES (NULL,'Jolyn Christen','LANZADOR',20,17,0,NULL,NULL,1.18,NULL);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>